<commit_message>
Added Changes for API ShortVisit
</commit_message>
<xml_diff>
--- a/doc/API_END_POINTS.xlsx
+++ b/doc/API_END_POINTS.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="32">
   <si>
     <t>API URL</t>
   </si>
@@ -81,9 +81,6 @@
     <t>/short_urls/:shorty</t>
   </si>
   <si>
-    <t>GET[HTTP]</t>
-  </si>
-  <si>
     <t>:shorty =&gt; Short URL</t>
   </si>
   <si>
@@ -106,6 +103,18 @@
   </si>
   <si>
     <t>GEO Location Details</t>
+  </si>
+  <si>
+    <t>/:shorty</t>
+  </si>
+  <si>
+    <t>/:shorty/geo_detail?page=:page_num</t>
+  </si>
+  <si>
+    <t>:shorty =&gt; Short URL, :page_num =&gt; Current page Number</t>
+  </si>
+  <si>
+    <t>GET[HTTP/API]</t>
   </si>
 </sst>
 </file>
@@ -121,12 +130,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="16"/>
-      <color rgb="FF333333"/>
-      <name val="Helvetica"/>
-    </font>
-    <font>
       <sz val="16"/>
       <color rgb="FF333333"/>
       <name val="Helvetica"/>
@@ -134,18 +137,48 @@
     <font>
       <u/>
       <sz val="12"/>
-      <color theme="10"/>
+      <color theme="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color rgb="FFFFFF00"/>
+      <name val="Helvetica"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCCFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -157,18 +190,30 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="7">
+    <cellStyle name="Followed Hyperlink" xfId="1" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -501,7 +546,7 @@
   <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -542,16 +587,16 @@
     </row>
     <row r="3" spans="1:4" ht="17">
       <c r="A3" s="2" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>11</v>
+        <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="17">
@@ -569,94 +614,106 @@
       </c>
     </row>
     <row r="5" spans="1:4" ht="17">
-      <c r="A5" s="2" t="s">
+      <c r="A5" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="17">
+      <c r="A6" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="17">
+      <c r="A7" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="17">
+      <c r="A8" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B8" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="C8" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="D8" s="4" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="17">
-      <c r="A6" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B6" s="2" t="s">
+    <row r="9" spans="1:4" ht="17">
+      <c r="A9" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B9" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="17">
-      <c r="A7" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B7" s="2" t="s">
+      <c r="C9" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C7" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" ht="17">
-      <c r="A8" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="17">
-      <c r="A9" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>26</v>
+      <c r="D9" s="4" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="17">
-      <c r="A10" s="2" t="s">
+      <c r="A10" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="D10" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="B10" s="2" t="s">
+    </row>
+    <row r="11" spans="1:4" ht="17">
+      <c r="A11" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B11" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C10" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4">
-      <c r="A11" s="3"/>
+      <c r="C11" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>11</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>